<commit_message>
comit before major refactor
</commit_message>
<xml_diff>
--- a/packages/ether-backend/0-PROJECT/Chifre.xlsx
+++ b/packages/ether-backend/0-PROJECT/Chifre.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHARED\WORKSPACE\projects\millionr.club\packages\ether-backend\0-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{385C7130-D8EF-4DF5-A609-853504F8D1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF535D87-C9B5-42F4-814B-749AE9691EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C95A2660-8DA4-4999-BA7B-977E40AD84A8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C95A2660-8DA4-4999-BA7B-977E40AD84A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Membership</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>Revenu - Ma cote</t>
+  </si>
+  <si>
+    <t>VIP Members</t>
+  </si>
+  <si>
+    <t>More rewards exclusive for them</t>
+  </si>
+  <si>
+    <t>2 chance instead of 1 on Big price</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B9784AF-1617-4F15-BD8C-E9FA575D46CB}">
-  <dimension ref="B6:N34"/>
+  <dimension ref="B6:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +932,7 @@
       <c r="N31" s="5"/>
     </row>
     <row r="32" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
         <v>0</v>
       </c>
@@ -937,7 +946,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="13">
         <v>10000</v>
       </c>
@@ -965,7 +974,23 @@
         <v>5250000</v>
       </c>
     </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>